<commit_message>
Add Google-style progress bar to scoreboard during live game
Elastic oscillating progress bar below Q1-Q4 quarter pills
when game is live and quarters still in progress. Uses Material
Design cubic-bezier easing with width morphing for authentic
Google-style motion. Adapts to theme/team primary color.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SBSquares_Task_Report.xlsx
+++ b/SBSquares_Task_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinivaskoduri/SBSquares/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6862363E-F65D-8E42-A4B9-800807E0CBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F1A1B0-7D64-6342-9031-40DB5BD077E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="68480" windowHeight="26280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="86">
   <si>
     <t>Task #</t>
   </si>
@@ -244,6 +244,15 @@
     <t>Add admin ability to edit team names with safety checks</t>
   </si>
   <si>
+    <t>Create Help / How to Play page at /help</t>
+  </si>
+  <si>
+    <t>app/help/page.tsx, app/page.tsx, app/game/[gameId]/page.tsx</t>
+  </si>
+  <si>
+    <t>Sliding number digits use theme/team primary color + deploy</t>
+  </si>
+  <si>
     <t>Summary</t>
   </si>
   <si>
@@ -262,7 +271,10 @@
     <t>1/1 completed</t>
   </si>
   <si>
-    <t>24/24 completed</t>
+    <t>6/6 completed</t>
+  </si>
+  <si>
+    <t>25/25 completed</t>
   </si>
   <si>
     <t>By Type</t>
@@ -667,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B37"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1361,7 +1373,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>39</v>
       </c>
@@ -1381,7 +1393,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>40</v>
       </c>
@@ -1401,7 +1413,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>41</v>
       </c>
@@ -1421,85 +1433,101 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
+    <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>43</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="C38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>44</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="6">
-        <v>36</v>
-      </c>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="6">
-        <v>36</v>
-      </c>
+      <c r="A41" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
+      <c r="A42" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="6">
+        <v>38</v>
+      </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="6"/>
+      <c r="A43" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="6">
+        <v>38</v>
+      </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>79</v>
-      </c>
+      <c r="A45" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -1507,10 +1535,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -1519,10 +1547,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -1531,10 +1559,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
@@ -1542,42 +1570,42 @@
       <c r="F48" s="6"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
+      <c r="A49" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B50" s="6"/>
+      <c r="A50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B51" s="6">
-        <v>6</v>
-      </c>
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="6">
-        <v>1</v>
-      </c>
+      <c r="A52" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -1585,10 +1613,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B53" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
@@ -1597,10 +1625,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B54" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
@@ -1609,10 +1637,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B55" s="6">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
@@ -1621,10 +1649,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B56" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
@@ -1633,10 +1661,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B57" s="6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -1644,12 +1672,56 @@
       <c r="F57" s="6"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="A58" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="6">
+        <v>4</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="6">
+        <v>2</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B58">
+      <c r="B60" s="6">
         <v>1</v>
       </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: add game limit (max 20) and superadmin dashboard for free-tier safeguards
- Enforce max 20 game limit with count check before game creation
- Add /superadmin dashboard with PIN auth (server-side API route)
- Dashboard shows all games with status, player count, squares picked, time ago
- Cascade delete games from superadmin with confirmation dialog
- Add QR code copy/download buttons to admin invite section
- Update task tracker with tasks #94-#99

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SBSquares_Task_Report.xlsx
+++ b/SBSquares_Task_Report.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -45,6 +45,11 @@
     <font/>
     <font>
       <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -95,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -116,6 +121,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
@@ -2725,239 +2731,362 @@
         </is>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" s="10" t="n">
+        <v>94</v>
+      </c>
+      <c r="B76" s="10" t="inlineStr">
+        <is>
+          <t>Design game limit and superadmin safeguards</t>
+        </is>
+      </c>
+      <c r="C76" s="10" t="inlineStr">
+        <is>
+          <t>Architecture</t>
+        </is>
+      </c>
+      <c r="D76" s="10" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="E76" s="10" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F76" s="10" t="inlineStr">
+        <is>
+          <t>N/A (design document)</t>
+        </is>
+      </c>
+    </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Summary</t>
+      <c r="A77" s="10" t="n">
+        <v>95</v>
+      </c>
+      <c r="B77" s="10" t="inlineStr">
+        <is>
+          <t>Add game creation limit (max 20) to landing page</t>
+        </is>
+      </c>
+      <c r="C77" s="10" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D77" s="10" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E77" s="10" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F77" s="10" t="inlineStr">
+        <is>
+          <t>app/page.tsx, lib/constants.ts</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Total Tasks:</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>73</v>
+      <c r="A78" s="10" t="n">
+        <v>96</v>
+      </c>
+      <c r="B78" s="10" t="inlineStr">
+        <is>
+          <t>Create superadmin PIN verification API route</t>
+        </is>
+      </c>
+      <c r="C78" s="10" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D78" s="10" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E78" s="10" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F78" s="10" t="inlineStr">
+        <is>
+          <t>app/api/superadmin/verify/route.ts, .env.local</t>
+        </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Completed:</t>
-        </is>
-      </c>
-      <c r="B79" t="n">
-        <v>73</v>
+      <c r="A79" s="10" t="n">
+        <v>97</v>
+      </c>
+      <c r="B79" s="10" t="inlineStr">
+        <is>
+          <t>Build superadmin dashboard page</t>
+        </is>
+      </c>
+      <c r="C79" s="10" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D79" s="10" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E79" s="10" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F79" s="10" t="inlineStr">
+        <is>
+          <t>app/superadmin/page.tsx, lib/utils.ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="10" t="n">
+        <v>98</v>
+      </c>
+      <c r="B80" s="10" t="inlineStr">
+        <is>
+          <t>Create dummy test data for game limit testing</t>
+        </is>
+      </c>
+      <c r="C80" s="10" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="D80" s="10" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E80" s="10" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F80" s="10" t="inlineStr">
+        <is>
+          <t>N/A (test data)</t>
+        </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>By Assignee</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
+      <c r="A81" s="10" t="n">
+        <v>99</v>
+      </c>
+      <c r="B81" s="10" t="inlineStr">
+        <is>
+          <t>Verify cascade delete and game limit enforcement</t>
+        </is>
+      </c>
+      <c r="C81" s="10" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="D81" s="10" t="inlineStr">
         <is>
           <t>architect</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>5/5 completed</t>
-        </is>
-      </c>
-    </row>
+      <c r="E81" s="10" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F81" s="10" t="inlineStr">
+        <is>
+          <t>N/A (verification)</t>
+        </is>
+      </c>
+    </row>
+    <row r="82"/>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>architect + team-lead-2</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>1/1 completed</t>
+          <t>Summary</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>backend-dev</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>10/10 completed</t>
-        </is>
+          <t>Total Tasks:</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>devops</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>2/2 completed</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>devops + team-lead-2</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>1/1 completed</t>
-        </is>
-      </c>
-    </row>
+          <t>Completed:</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86"/>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>team-lead</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>1/1 completed</t>
+          <t>By Assignee</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>team-lead-2</t>
+          <t>architect</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>13/13 completed</t>
+          <t>7/7 completed</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>uat-tester</t>
+          <t>architect + team-lead-2</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>6/6 completed</t>
+          <t>1/1 completed</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>ui-dev</t>
+          <t>backend-dev</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>34/34 completed</t>
+          <t>10/10 completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>devops</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2/2 completed</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>By Type</t>
+          <t>devops + team-lead-2</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>1/1 completed</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Architecture</t>
-        </is>
-      </c>
-      <c r="B93" t="n">
-        <v>4</v>
+          <t>team-lead</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>1/1 completed</t>
+        </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Bug Fix</t>
-        </is>
-      </c>
-      <c r="B94" t="n">
-        <v>13</v>
+          <t>team-lead-2</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>13/13 completed</t>
+        </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Config</t>
-        </is>
-      </c>
-      <c r="B95" t="n">
-        <v>1</v>
+          <t>uat-tester</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>6/6 completed</t>
+        </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>DevOps</t>
-        </is>
-      </c>
-      <c r="B96" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>Enhancement</t>
-        </is>
-      </c>
-      <c r="B97" t="n">
-        <v>11</v>
-      </c>
-    </row>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>37/37 completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="97"/>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="B98" t="n">
-        <v>20</v>
+          <t>By Type</t>
+        </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Migration</t>
+          <t>Architecture</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Research</t>
+          <t>Bug Fix</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Review</t>
+          <t>Config</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -2967,31 +3096,101 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>UAT</t>
+          <t>DevOps</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>UI Fix</t>
+          <t>Enhancement</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Migration</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>UAT</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>UI Fix</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
           <t>UI Redesign</t>
         </is>
       </c>
-      <c r="B104" t="n">
+      <c r="B110" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: support all 32 NFL teams with autocomplete team selector
- Add NFL_TEAMS master list (32 teams with name, city, abbreviation, colors)
- TeamCombobox: filterable dropdown with logos, keyboard nav, custom name support
- TeamLogo.tsx now supports all 32 teams via ESPN CDN
- use-theme.ts expanded from 8 to 32 team color palettes
- Replace free-text team inputs in game creation and admin editing
- Prevent duplicate team selection (same team for row and col)

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SBSquares_Task_Report.xlsx
+++ b/SBSquares_Task_Report.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
@@ -3035,308 +3035,600 @@
         </is>
       </c>
     </row>
-    <row r="86"/>
+    <row r="86">
+      <c r="A86" s="6" t="n">
+        <v>105</v>
+      </c>
+      <c r="B86" s="6" t="inlineStr">
+        <is>
+          <t>Add all 32 NFL teams master list to lib/constants.ts</t>
+        </is>
+      </c>
+      <c r="C86" s="6" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D86" s="6" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E86" s="6" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F86" s="6" t="inlineStr">
+        <is>
+          <t>lib/constants.ts</t>
+        </is>
+      </c>
+    </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>Summary</t>
+      <c r="A87" s="6" t="n">
+        <v>106</v>
+      </c>
+      <c r="B87" s="6" t="inlineStr">
+        <is>
+          <t>Update TeamLogo.tsx to use NFL_TEAMS from constants (all 32 teams)</t>
+        </is>
+      </c>
+      <c r="C87" s="6" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D87" s="6" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E87" s="6" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F87" s="6" t="inlineStr">
+        <is>
+          <t>components/TeamLogo.tsx</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>Total Tasks:</t>
-        </is>
-      </c>
-      <c r="B88" t="n">
-        <v>84</v>
+      <c r="A88" s="6" t="n">
+        <v>107</v>
+      </c>
+      <c r="B88" s="6" t="inlineStr">
+        <is>
+          <t>Add color palettes for all 32 NFL teams in use-theme.ts</t>
+        </is>
+      </c>
+      <c r="C88" s="6" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D88" s="6" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E88" s="6" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F88" s="6" t="inlineStr">
+        <is>
+          <t>hooks/use-theme.ts</t>
+        </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>Completed:</t>
-        </is>
-      </c>
-      <c r="B89" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="90"/>
+      <c r="A89" s="6" t="n">
+        <v>108</v>
+      </c>
+      <c r="B89" s="6" t="inlineStr">
+        <is>
+          <t>Design TeamCombobox UX specification</t>
+        </is>
+      </c>
+      <c r="C89" s="6" t="inlineStr">
+        <is>
+          <t>UX</t>
+        </is>
+      </c>
+      <c r="D89" s="6" t="inlineStr">
+        <is>
+          <t>ux-expert</t>
+        </is>
+      </c>
+      <c r="E89" s="6" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F89" s="6" t="inlineStr">
+        <is>
+          <t>N/A (design spec)</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="6" t="n">
+        <v>109</v>
+      </c>
+      <c r="B90" s="6" t="inlineStr">
+        <is>
+          <t>Build TeamCombobox component with filtered dropdown and logo preview</t>
+        </is>
+      </c>
+      <c r="C90" s="6" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D90" s="6" t="inlineStr">
+        <is>
+          <t>team-lead-2</t>
+        </is>
+      </c>
+      <c r="E90" s="6" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F90" s="6" t="inlineStr">
+        <is>
+          <t>components/TeamCombobox.tsx</t>
+        </is>
+      </c>
+    </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>By Assignee</t>
+      <c r="A91" s="6" t="n">
+        <v>110</v>
+      </c>
+      <c r="B91" s="6" t="inlineStr">
+        <is>
+          <t>Replace team inputs in game creation form with TeamCombobox</t>
+        </is>
+      </c>
+      <c r="C91" s="6" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D91" s="6" t="inlineStr">
+        <is>
+          <t>team-lead-2</t>
+        </is>
+      </c>
+      <c r="E91" s="6" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F91" s="6" t="inlineStr">
+        <is>
+          <t>app/page.tsx</t>
         </is>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>architect</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>7/7 completed</t>
+      <c r="A92" s="6" t="n">
+        <v>111</v>
+      </c>
+      <c r="B92" s="6" t="inlineStr">
+        <is>
+          <t>Replace team inputs in admin page with TeamCombobox</t>
+        </is>
+      </c>
+      <c r="C92" s="6" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D92" s="6" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E92" s="6" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F92" s="6" t="inlineStr">
+        <is>
+          <t>app/game/[gameId]/admin/page.tsx</t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>architect + team-lead-2</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>1/1 completed</t>
+      <c r="A93" s="6" t="n">
+        <v>112</v>
+      </c>
+      <c r="B93" s="6" t="inlineStr">
+        <is>
+          <t>Add city field to NFL_TEAMS and city search in TeamCombobox</t>
+        </is>
+      </c>
+      <c r="C93" s="6" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D93" s="6" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E93" s="6" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F93" s="6" t="inlineStr">
+        <is>
+          <t>lib/constants.ts, components/TeamCombobox.tsx</t>
         </is>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>backend-dev</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>10/10 completed</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>devops</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>2/2 completed</t>
-        </is>
-      </c>
-    </row>
+      <c r="A94" s="6" t="n">
+        <v>113</v>
+      </c>
+      <c r="B94" s="6" t="inlineStr">
+        <is>
+          <t>Prevent duplicate team selection (same team for row and col)</t>
+        </is>
+      </c>
+      <c r="C94" s="6" t="inlineStr">
+        <is>
+          <t>Bug Fix</t>
+        </is>
+      </c>
+      <c r="D94" s="6" t="inlineStr">
+        <is>
+          <t>orchestrator</t>
+        </is>
+      </c>
+      <c r="E94" s="6" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F94" s="6" t="inlineStr">
+        <is>
+          <t>app/page.tsx, app/game/[gameId]/admin/page.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="95"/>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>devops + team-lead-2</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>1/1 completed</t>
+          <t>Summary</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>team-lead</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>1/1 completed</t>
-        </is>
+          <t>Total Tasks:</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>93</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>team-lead-2</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>13/13 completed</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>uat-tester</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>6/6 completed</t>
-        </is>
-      </c>
-    </row>
+          <t>Completed:</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99"/>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>ui-dev</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>37/37 completed</t>
+          <t>By Assignee</t>
         </is>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="7" t="inlineStr">
-        <is>
-          <t>orchestrator</t>
-        </is>
-      </c>
-      <c r="B101" s="7" t="inlineStr">
-        <is>
-          <t>5/5 completed</t>
-        </is>
-      </c>
-    </row>
-    <row r="102"/>
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>7/7 completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>architect + team-lead-2</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>1/1 completed</t>
+        </is>
+      </c>
+    </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>By Type</t>
+          <t>backend-dev</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>10/10 completed</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Architecture</t>
-        </is>
-      </c>
-      <c r="B104" t="n">
-        <v>5</v>
+          <t>devops</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>2/2 completed</t>
+        </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Bug Fix</t>
-        </is>
-      </c>
-      <c r="B105" t="n">
-        <v>14</v>
+          <t>devops + team-lead-2</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>1/1 completed</t>
+        </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Config</t>
-        </is>
-      </c>
-      <c r="B106" t="n">
-        <v>1</v>
+          <t>team-lead</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>1/1 completed</t>
+        </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>DevOps</t>
-        </is>
-      </c>
-      <c r="B107" t="n">
-        <v>5</v>
+          <t>team-lead-2</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>15/15 completed</t>
+        </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Enhancement</t>
-        </is>
-      </c>
-      <c r="B108" t="n">
-        <v>11</v>
+          <t>uat-tester</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>6/6 completed</t>
+        </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="B109" t="n">
-        <v>24</v>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>42/42 completed</t>
+        </is>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>Migration</t>
-        </is>
-      </c>
-      <c r="B110" t="n">
-        <v>1</v>
+      <c r="A110" s="7" t="inlineStr">
+        <is>
+          <t>orchestrator</t>
+        </is>
+      </c>
+      <c r="B110" s="7" t="inlineStr">
+        <is>
+          <t>6/6 completed</t>
+        </is>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>Research</t>
-        </is>
-      </c>
-      <c r="B111" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="B112" t="n">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="A111" s="7" t="inlineStr">
+        <is>
+          <t>ux-expert</t>
+        </is>
+      </c>
+      <c r="B111" s="7" t="inlineStr">
+        <is>
+          <t>1/1 completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="112"/>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>UAT</t>
-        </is>
-      </c>
-      <c r="B113" t="n">
-        <v>6</v>
+          <t>By Type</t>
+        </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>UI Fix</t>
+          <t>Architecture</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>UI Redesign</t>
+          <t>Bug Fix</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
+          <t>Config</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>DevOps</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Migration</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>UAT</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>UI Fix</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>UI Redesign</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
           <t>Testing</t>
         </is>
       </c>
-      <c r="B116" t="n">
+      <c r="B126" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" s="7" t="inlineStr">
+    <row r="127">
+      <c r="A127" s="7" t="inlineStr">
         <is>
           <t>Docs</t>
         </is>
       </c>
-      <c r="B117" s="7" t="n">
+      <c r="B127" s="7" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="7" t="inlineStr">
+        <is>
+          <t>UX</t>
+        </is>
+      </c>
+      <c r="B128" s="7" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add automatic live score updates from ESPN
Poll ESPN's public scoreboard API every 30s during live games to
auto-update quarter scores, calculate winners, and broadcast via
Supabase realtime. Admin toggle in Score Entry enables/disables
auto-pilot mode. Includes Super Bowl auto-detect, adaptive polling
intervals, overtime handling, and summary endpoint fallback for
historical games.

New files:
- lib/espn.ts (ESPN API client with cumulative score mapping)
- app/api/live-scores/route.ts (score polling + Supabase upsert)
- app/api/live-scores/detect/route.ts (Super Bowl auto-detect)
- hooks/use-live-scores.ts (adaptive 30s/60s client polling)
- supabase/migrations/20250207000000_live_scores.sql

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SBSquares_Task_Report.xlsx
+++ b/SBSquares_Task_Report.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
@@ -3305,296 +3305,548 @@
         </is>
       </c>
     </row>
-    <row r="95"/>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>114</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Add auto_scores_enabled and espn_event_id columns to games table + update TypeScript types</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Migration</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>supabase/migrations/20250207000000_live_scores.sql, lib/types.ts</t>
+        </is>
+      </c>
+    </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>Summary</t>
+      <c r="A96" t="n">
+        <v>115</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Build ESPN API client with scoreboard fetch, game parser, team finder, and team-axis matcher</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>lib/espn.ts</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>Total Tasks:</t>
-        </is>
-      </c>
-      <c r="B97" t="n">
-        <v>93</v>
+      <c r="A97" t="n">
+        <v>116</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Create live-scores API route with ESPN polling, score mapping, and Supabase upserts</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>app/api/live-scores/route.ts</t>
+        </is>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>Completed:</t>
-        </is>
-      </c>
-      <c r="B98" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="99"/>
+      <c r="A98" t="n">
+        <v>117</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Create client-side polling hook with adaptive intervals (30s live, 60s idle)</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>hooks/use-live-scores.ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>118</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Add auto-update ESPN toggle, NFL status indicator, and disable manual inputs in ScoreEntry</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>app/game/[gameId]/admin/page.tsx</t>
+        </is>
+      </c>
+    </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>By Assignee</t>
+      <c r="A100" t="n">
+        <v>119</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Research NFL live score APIs (ESPN public scoreboard, no auth required)</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>product-researcher</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>N/A (research only)</t>
         </is>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
+      <c r="A101" t="n">
+        <v>120</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Create architecture plan for live score auto-update feature (data flow, file list, edge cases)</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Docs</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
         <is>
           <t>architect</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>7/7 completed</t>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>N/A (architecture plan)</t>
         </is>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>architect + team-lead-2</t>
-        </is>
+      <c r="A102" t="n">
+        <v>121</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>1/1 completed</t>
+          <t>Add Super Bowl auto-detect endpoint using ESPN scoreboard date filtering and team matching</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>app/api/live-scores/detect/route.ts, lib/espn.ts</t>
         </is>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>backend-dev</t>
-        </is>
+      <c r="A103" t="n">
+        <v>122</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>10/10 completed</t>
+          <t>Fix ESPN fetchESPNScores to fallback to summary endpoint for historical games</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Bugfix</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>team-lead-2</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>lib/espn.ts</t>
         </is>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>devops</t>
-        </is>
+      <c r="A104" t="n">
+        <v>123</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2/2 completed</t>
+          <t>Free tier safety analysis for live score polling (30s interval confirmed safe)</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>N/A (analysis only)</t>
         </is>
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>devops + team-lead-2</t>
-        </is>
+      <c r="A105" t="n">
+        <v>124</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>1/1 completed</t>
+          <t>Add live score polling free tier analysis to research findings doc</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Docs</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>product-researcher</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>docs/research-findings.md</t>
         </is>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>team-lead</t>
-        </is>
+      <c r="A106" t="n">
+        <v>125</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>1/1 completed</t>
+          <t>Add Session 5 agent team success story to README</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Docs</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>README.md</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>team-lead-2</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>15/15 completed</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>uat-tester</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>6/6 completed</t>
-        </is>
-      </c>
-    </row>
+          <t>Completed:</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="108"/>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>ui-dev</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>42/42 completed</t>
+          <t>By Assignee</t>
         </is>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="7" t="inlineStr">
-        <is>
-          <t>orchestrator</t>
-        </is>
-      </c>
-      <c r="B110" s="7" t="inlineStr">
-        <is>
-          <t>6/6 completed</t>
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>7/7 completed</t>
         </is>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="7" t="inlineStr">
-        <is>
-          <t>ux-expert</t>
-        </is>
-      </c>
-      <c r="B111" s="7" t="inlineStr">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>architect + team-lead-2</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
         <is>
           <t>1/1 completed</t>
         </is>
       </c>
     </row>
-    <row r="112"/>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>backend-dev</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>10/10 completed</t>
+        </is>
+      </c>
+    </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>By Type</t>
+          <t>devops</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>2/2 completed</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Architecture</t>
-        </is>
-      </c>
-      <c r="B114" t="n">
-        <v>5</v>
+          <t>devops + team-lead-2</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>1/1 completed</t>
+        </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Bug Fix</t>
-        </is>
-      </c>
-      <c r="B115" t="n">
-        <v>15</v>
+          <t>team-lead</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>1/1 completed</t>
+        </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Config</t>
-        </is>
-      </c>
-      <c r="B116" t="n">
-        <v>1</v>
+          <t>team-lead-2</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>15/15 completed</t>
+        </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>DevOps</t>
-        </is>
-      </c>
-      <c r="B117" t="n">
-        <v>5</v>
+          <t>uat-tester</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>6/6 completed</t>
+        </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Enhancement</t>
-        </is>
-      </c>
-      <c r="B118" t="n">
-        <v>16</v>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>42/42 completed</t>
+        </is>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="B119" t="n">
-        <v>26</v>
+      <c r="A119" s="7" t="inlineStr">
+        <is>
+          <t>orchestrator</t>
+        </is>
+      </c>
+      <c r="B119" s="7" t="inlineStr">
+        <is>
+          <t>6/6 completed</t>
+        </is>
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>Migration</t>
-        </is>
-      </c>
-      <c r="B120" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>Research</t>
-        </is>
-      </c>
-      <c r="B121" t="n">
-        <v>8</v>
-      </c>
-    </row>
+      <c r="A120" s="7" t="inlineStr">
+        <is>
+          <t>ux-expert</t>
+        </is>
+      </c>
+      <c r="B120" s="7" t="inlineStr">
+        <is>
+          <t>1/1 completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="121"/>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="B122" t="n">
-        <v>1</v>
+          <t>By Type</t>
+        </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>UAT</t>
+          <t>Architecture</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>UI Fix</t>
+          <t>Bug Fix</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>UI Redesign</t>
+          <t>Config</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -3604,30 +3856,120 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
+          <t>DevOps</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Migration</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>UAT</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>UI Fix</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>UI Redesign</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
           <t>Testing</t>
         </is>
       </c>
-      <c r="B126" t="n">
+      <c r="B135" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" s="7" t="inlineStr">
+    <row r="136">
+      <c r="A136" s="7" t="inlineStr">
         <is>
           <t>Docs</t>
         </is>
       </c>
-      <c r="B127" s="7" t="n">
+      <c r="B136" s="7" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="128">
-      <c r="A128" s="7" t="inlineStr">
+    <row r="137">
+      <c r="A137" s="7" t="inlineStr">
         <is>
           <t>UX</t>
         </is>
       </c>
-      <c r="B128" s="7" t="n">
+      <c r="B137" s="7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: improve QR join flow, add system theme toggle, fix grid cell visibility
- QR code /join page now redirects returning players to their game view
- When game is not accepting players, /join redirects to /?code= for sign-in
- Show game code reminder toast after joining via QR for future reference
- Add 3-segment theme toggle (dark/light/system) with OS preference tracking
- Update FOUC prevention script to handle system theme preference
- Improve self-pick grid cell borders in dark mode with solid colors and glow
- Add lightenColor utility for per-color brightness adjustment

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SBSquares_Task_Report.xlsx
+++ b/SBSquares_Task_Report.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
@@ -3973,6 +3973,156 @@
         <v>1</v>
       </c>
     </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>126</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>QR code session redirect — redirect returning players to game view</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>app/join/[gameCode]/page.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>127</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Game code reminder toast after joining via QR</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>app/join/[gameCode]/page.tsx, app/game/[gameId]/page.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>128</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Redirect /join to /?code= when game not accepting players</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>app/join/[gameCode]/page.tsx, app/page.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>129</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Add system theme option with 3-segment toggle (dark/light/system)</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>hooks/use-theme.ts, app/layout.tsx, app/game/[gameId]/page.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>130</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Improve grid cell border visibility in dark mode</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>components/GridCell.tsx, components/Grid.tsx, lib/utils.ts</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add tentative pick flow with confirm/cancel, timer, and admin tools
Implement a tentative pick system for the draft phase where players
select squares that are staged (visible to all in real-time) before
being finalized on confirm. Includes a 2-minute countdown timer with
automatic random-fill on timeout.

Key changes:
- Tentative pick queue with circular replacement and ref-based mutex
- Floating bottom bar UI with dot indicators, timer, and confirm button
- Visual states for tentative squares (pulse ring, numbered badges)
- Admin tools: tentative cleanup, Selecting indicators, square reassign
- Defensive checks excluding tentative squares from winner calc
- Migration: is_tentative on squares, tentative_started_at on draft_order

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SBSquares_Task_Report.xlsx
+++ b/SBSquares_Task_Report.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
@@ -3675,7 +3675,6 @@
         <v>93</v>
       </c>
     </row>
-    <row r="108"/>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
@@ -3815,7 +3814,6 @@
         </is>
       </c>
     </row>
-    <row r="121"/>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
@@ -4120,6 +4118,456 @@
       <c r="F142" t="inlineStr">
         <is>
           <t>components/GridCell.tsx, components/Grid.tsx, lib/utils.ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>20</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>feature</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Floating bottom bar for tentative pick UI (PickControls manual mode redesign, info/warning toasts, grid padding)</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>21</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>bugfix</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Replace pick toasts with modals (info toast firing repeatedly, 30s warning not prominent enough)</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>145</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>bugfix</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Fix dot indicator count showing x/10 instead of x/5 - totalPicks was picksUsed+picksRemaining (double counting tentative picks), changed to picksRemaining only</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>146</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>bugfix</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Fix timeout handler stale closure and over-filling - added handleTimeoutRef for latest closure, re-fetches fresh squares from DB instead of stale state, added Math.max(0,...) safety cap</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>147</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>bugfix</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Add mutex lock (pickingRef) to handleTentativePick to prevent race condition from fast double-clicks</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>131</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Enhanced grid cell visibility (solid borders, glow, thicker width for self-picks in dark mode)</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>components/GridCell.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>132</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Schema migration: add is_tentative and tentative_started_at columns for tentative picks</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>supabase/schema.sql, supabase/migrations/20250208000000_tentative_picks.sql, lib/game-logic.ts, app/api/live-scores/route.ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>133</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Implement tentative pick logic with circular replacement queue and 2-min timer</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>app/game/[gameId]/page.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>134</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Update Grid and GridCell for tentative pick visual states (pulsing ring, pick number badges)</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>components/Grid.tsx, components/GridCell.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>135</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Update PickControls with confirm button, countdown timer, and floating bottom bar</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>components/PickControls.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>136</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Update admin page for tentative pick cleanup (pickOnBehalf, resetGame, clearPlayerPicks)</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>app/game/[gameId]/admin/page.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>137</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Debug tentative picks failure - root cause: migration not applied to deployed DB</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Bug Fix</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>architect + ui-dev</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>N/A (migration deployment)</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>138</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Fix maxPicks derivation using getDraftConfig instead of stale picks_remaining</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Bug Fix</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>app/game/[gameId]/page.tsx, components/PickControls.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>139</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Build admin square reassign feature with mini-grid and player dropdown</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>app/game/[gameId]/admin/page.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>140</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Add ref-based mutex to handleRandomPick to prevent double-fire race condition</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Bug Fix</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>components/PickControls.tsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>158</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>bugfix</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Add ref-based mutex to handleRandomPick in PickControls to prevent double-fire via devtools bypass</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Done</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add live score pulsing squares with simulation testing
Show pulsing gold/silver glow on grid squares that are currently winning
during in-progress NFL quarters. Squares bounce around as teams score,
then lock in with solid rings when quarters complete.

- Add live_quarter_score JSONB column to games table
- API route writes in-progress quarter scores from ESPN data
- Grid computes live winner/runner-up using digit assignments
- Pulsing CSS animations (1.5s gold/silver glow cycles)
- ScoreBoard shows live ESPN status detail and score shimmer
- Simulation system with 20-step Super Bowl LIX fixture for testing
- Dev-only simulation runner in admin panel (Next Step / Auto / Reset)
- Fix: live pulsing overlays confirmed winners from earlier quarters
- Bump all badge font sizes to 10px for mobile readability

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SBSquares_Task_Report.xlsx
+++ b/SBSquares_Task_Report.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:F165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
@@ -3675,6 +3675,7 @@
         <v>93</v>
       </c>
     </row>
+    <row r="108"/>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
@@ -3814,6 +3815,7 @@
         </is>
       </c>
     </row>
+    <row r="121"/>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
@@ -4566,6 +4568,181 @@
         </is>
       </c>
       <c r="E158" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>159</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>feature</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Live Score Pulsing Squares - DB migration (live_quarter_score JSONB column)</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>architect</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>160</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>feature</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Live Score Pulsing Squares - CSS pulsing animations + ScoreBoard live display</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>uiux-expert</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>161</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>feature</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Live Score Pulsing Squares - Grid/GridCell live winner/runner-up pulsing logic</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>ui-dev-1</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>162</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>feature</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Live Score Pulsing Squares - Simulation system (API + fixture + admin runner)</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>ui-dev-2</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>163</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>bugfix</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Live Score Pulsing Squares - Fix duplicate type in ScoreBoard, final review + build</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>team-lead</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>164</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>bugfix</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Live pulsing: allow LIVE badge on squares that are already confirmed winners from earlier quarters</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Srini</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>165</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>bugfix</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Increase badge font sizes (winner/runner-up/LIVE/tentative) from 5-8px to 10px for mobile readability</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Srini</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
         <is>
           <t>Done</t>
         </is>

</xml_diff>

<commit_message>
fix: resolve race condition in admin draft pick-on-behalf + add plan docs
Admin rapid-clicking "pick for user" across multiple players caused stale
React state to generate overlapping random picks, leaving some players with
fewer squares than expected. Fix adds promise-based queue to serialize pick
operations, fresh DB reads before each pick, verified writes with retry,
and UI guards (all buttons disabled during any pick, queue indicators, toasts).

Also adds future plan documents for Turnstile CAPTCHA and server-side live scores.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SBSquares_Task_Report.xlsx
+++ b/SBSquares_Task_Report.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F165"/>
+  <dimension ref="A1:F171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
@@ -3675,7 +3675,6 @@
         <v>93</v>
       </c>
     </row>
-    <row r="108"/>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
@@ -3815,7 +3814,6 @@
         </is>
       </c>
     </row>
-    <row r="121"/>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
@@ -4745,6 +4743,166 @@
       <c r="E165" t="inlineStr">
         <is>
           <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>166</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>feature</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Gate simulation runner behind per-game simulation_enabled flag with superadmin toggle</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Srini</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>166</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>docs</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Create future plan document for server-side live score polling (pg_cron + pg_net)</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>167</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>docs</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Create future plan document for Cloudflare Turnstile CAPTCHA on game creation</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>docs/plan-turnstile-captcha.md</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>168</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>bugfix</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Fix draft pick race condition: serialize pickOnBehalf with promise queue, fetch fresh squares from DB, verify pick success counts, retry on contention, add queue/active UI indicators</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>169</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>feature</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Add UX feedback for draft pick operations: picking banner with spinner above draft circles, toast notifications on success/failure, disable ALL pick buttons during any active operation</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>ui-dev</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>168</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>bugfix</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Fix race condition in admin draft pick-on-behalf: promise queue + fresh DB reads + verify/retry + UI queue indicators</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Team (architect, uiux-expert, ui-dev)</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>app/game/[gameId]/admin/page.tsx</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: add Supabase query optimization plan
Analyzes 13 slow queries (realtime.list_changes at 97.9% of DB time)
with prioritized optimization steps: debounce reload, remove rarely-changed
tables from publication, state-conditional subscriptions, and long-term
Broadcast from Database migration.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SBSquares_Task_Report.xlsx
+++ b/SBSquares_Task_Report.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F171"/>
+  <dimension ref="A1:F172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
@@ -4906,6 +4906,36 @@
         </is>
       </c>
     </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>169</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>research</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Analyze 13 slow Supabase queries and create optimization plan document</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Team (architect, backend-dev)</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>docs/plan-query-optimization.md</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>